<commit_message>
input handler class and deliverables
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5dba5270548c4a21/Documents/COP4534/dsp3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahje\OneDrive\Documents\COP4534\dsp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{DD2AF5B2-53A1-4300-BC29-D4967614CE69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CC0D84C3-38E5-49A0-9B74-140A9AF50BB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FAA6CF-E57B-4B4B-BA6C-897C79A5A166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{EEE85143-B0DB-46C2-A7A0-5624D094C985}"/>
+    <workbookView xWindow="4680" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{EEE85143-B0DB-46C2-A7A0-5624D094C985}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t># Cities</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Percent of Optimal GA produced (%)</t>
+  </si>
+  <si>
+    <t>All Results experimented with 100 tours, 100 generations and 70% mutations</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FA2B4A-26EA-4977-964D-F2DF24179624}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +532,11 @@
         <v>2.3E-2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>